<commit_message>
Fixing issue in data and fixing third t test
</commit_message>
<xml_diff>
--- a/uni_augsburg_001/main_study/evaluation.xlsx
+++ b/uni_augsburg_001/main_study/evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365adessogroup-my.sharepoint.com/personal/torben_soennecken_adesso_de/Documents/Private/University/Elite/sem3/IDE/studie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luis.schweigard/dev/azubee/hypothesis-tests/uni_augsburg_001/main_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1019" documentId="11_AD4DB114E441178AC67DF455DE92F000693EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCD6ECEC-3EFE-43AE-8478-E141C1539051}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF87A1E-CCB5-A242-AE62-91ACAECBF853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-888" yWindow="1104" windowWidth="17280" windowHeight="10044" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9920" yWindow="4100" windowWidth="17280" windowHeight="10040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pretest" sheetId="1" r:id="rId1"/>
@@ -466,16 +466,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -492,7 +492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -517,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -577,7 +577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -594,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -611,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -628,7 +628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -645,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -662,7 +662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -679,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -713,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>4</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>4</v>
       </c>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>5</v>
       </c>
@@ -849,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>5</v>
       </c>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>5</v>
       </c>
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>5</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>6</v>
       </c>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>6</v>
       </c>
@@ -951,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>6</v>
       </c>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>6</v>
       </c>
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>6</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>7</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>7</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>7</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>7</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>7</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>8</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>8</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>8</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>8</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>8</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>9</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>9</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>9</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>9</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>9</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>10</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>10</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>10</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>10</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>10</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>11</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>11</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>11</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>11</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>11</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>12</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>12</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>12</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>12</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>12</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1048576" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1048576" s="2"/>
     </row>
   </sheetData>
@@ -1528,9 +1528,9 @@
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>4</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>4</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>5</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>5</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>5</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>5</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>6</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>6</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>6</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>6</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>6</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>7</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>7</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>7</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>7</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>7</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>8</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>8</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>8</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>8</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>8</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>9</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>9</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>9</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>9</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>9</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>10</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>10</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>10</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>10</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>10</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>11</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>11</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>11</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>11</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>11</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>12</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>12</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>12</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>12</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>12</v>
       </c>
@@ -2576,16 +2576,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4528FC88-CA52-4161-AF24-64B1BF872EF5}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2699,13 +2699,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937AE6EF-3337-4407-B52F-B64D3C917EB6}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -2839,9 +2839,9 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>7</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>8</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>9</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>10</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>11</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>12</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="4"/>

</xml_diff>